<commit_message>
Assignment 1 Duplicate Fix
</commit_message>
<xml_diff>
--- a/Assignment_1/ilanlar.xlsx
+++ b/Assignment_1/ilanlar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,33 +498,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MENDERES MH.DE 2+1 ÇİFT CEPHE ARAKAT 85 M2 ARAKAT KİRALIK DAİRE</t>
+          <t>Buca İktisat Fakültesi Arkası Arakat Kiralık 1+1Klimalı Daire</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Menderes Mah.</t>
+          <t>İzmir / Buca / Adatepe Mah.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14.000
+          <t>14.500
 TL</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>84 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>25 Yaşında</t>
+          <t>5 Yaşında</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -534,60 +534,55 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>31-10-2024</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-menderes-kiralik/daire/147777-163</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/151862-3</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Isıtma Yok</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Elektrik</t>
+          <t>Klima</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Menderes Mh. Öğrenciye Kiralık 4+1 130 M2 Teraslı Doğalgazlı Daire</t>
+          <t>ÜNİVERSİTE YAKINI 1+0 EŞYALI D.GAZLI MERKEZİ KONUMDA KİRALIK LÜKS DAİRELER</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Menderes Mah.</t>
+          <t>İzmir / Buca / Yaylacık Mah.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20.000
+          <t>12.000
 TL</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4 + 1</t>
+          <t>Stüdyo</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>130 m²</t>
+          <t>40 m²</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>25 Yaşında</t>
+          <t>7 Yaşında</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -597,17 +592,17 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>26-09-2024</t>
+          <t>08-11-2024</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-menderes-kiralik/daire/24511-9074</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-yaylacik-kiralik/daire/111716-1034</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -624,48 +619,48 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Buca Göksu Mah İnkılap İzban Dibi 3+1 120 M2 D.gazlı</t>
+          <t>ASLAN EMLAK BUCA KURUCEŞME DOĞAL ĞAZLI ASANSÖRLÜ KİRALIK DAİRE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Göksu Mah.</t>
+          <t>İzmir / Buca / Kuruçeşme Mah.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>14.000
+          <t>13.000
 TL</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>120 m²</t>
+          <t>70 m²</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>21 Yaşında</t>
+          <t>5 Yaşında</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Giriş Katı</t>
+          <t>1. Kat</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>10-11-2024</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-goksu-kiralik/daire/83461-581</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/26765-2808</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -675,55 +670,60 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Kombi</t>
+          <t>Kat Kaloriferi</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GÜNEŞ'TEN ŞİRİNYER İZBAN 9DK 1+1 50M ASANSÖR KLİMA GÜNEY CEPHE</t>
+          <t>MARKA'DAN H.AĞA BAHÇESİ YAKINI 3+1 BALKONLU D.GAZLI KİRALIK DAİR</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>İzmir / Buca / İnkılap Mah.</t>
+          <t>İzmir / Buca / Atatürk Mah.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>16.500
+          <t>30.000
 TL</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>49 m²</t>
+          <t>145 m²</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2 Yaşında</t>
+          <t>21 Yaşında</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>4. Kat</t>
+          <t>3. Kat</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>10-11-2024</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-inkilap-kiralik/daire/130324-802</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/71024-1090</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -734,18 +734,13 @@
       <c r="K5" t="inlineStr">
         <is>
           <t>Kombi</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SİTE İÇİ KİRALIK 3+1 145m2 ARAKAT DAİRE</t>
+          <t>BUCA ÇAMLIKULE MAH.'NDE EŞYASIZ KİRALIK DAİRE (2+0)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -755,38 +750,38 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>34.000
+          <t>18.000
 TL</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>2 + 0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>145 m²</t>
+          <t>75 m²</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>3 Yaşında</t>
+          <t>2 Yaşında</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>12. Kat</t>
+          <t>4. Kat</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>10-11-2024</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-mustafa-kemal-kiralik/daire/145608-91</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-mustafa-kemal-kiralik/daire/145065-70</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -796,133 +791,123 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Merkezi (Pay Ölçer)</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
+          <t>Yerden Isıtma</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Deniz emlak dan Buca'da Yenigün mahallesinde kiralık daire</t>
+          <t>MARKA'DAN ANACADDE&amp;KAMPÜS YAKINI EŞYALI KLİMALI KİRALIK DAİRE</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kozağaç Mah.</t>
+          <t>İzmir / Buca / Kuruçeşme Mah.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15.000
+          <t>13.000
 TL</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>130 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>16 Yaşında</t>
+          <t>2 Yaşında</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>4. Kat</t>
+          <t>2. Kat</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>10-11-2024</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kozagac-kiralik/daire/120009-3</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/71024-1048</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Kombi</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
+          <t>Klima</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BUCADA EŞYALI, ASANSÖRLÜ, DOĞALGAZLI,KLİMALI, DOKUZ EYLÜL ÜNİ YANI, 1+1 KİRALIK</t>
+          <t>OYAK BUCA 1. ETAP SİTESİNDE 3+1 KİRALIK ÜÇ CEPHELİ GENİŞ LÜKS DAİRE</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+          <t>İzmir / Buca / Aydoğdu Mah.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>25.000
+          <t>39.000
 TL</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>50 m²</t>
+          <t>146 m²</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>4 Yaşında</t>
+          <t>8 Yaşında</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>8. Kat</t>
+          <t>Zemin</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>07-11-2024</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/77173-1070</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-aydogdu-kiralik/daire/91937-13</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Kombi</t>
+          <t>Merkezi (Pay Ölçer)</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -934,48 +919,48 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kiralık Buca da Yiğitler Mah.3+1 110 m2 Doğalgazlı açık otoparkı olan merkez de bir daire</t>
+          <t>ÖZPA - BUCA TENİS KULÜBÜ YANI TERASLI 2+1 DOĞALGAZLI OTOPARKLI TERASLI SIFIR KİRALIK DUBLEKS DAİRE</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Yiğitler Mah.</t>
+          <t>İzmir / Buca / Gaziler Mah.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>20.000
+          <t>22.000
 TL</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>2 + 1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>110 m²</t>
+          <t>100 m²</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>7 Yaşında</t>
+          <t>Sıfır Bina</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Yarı Bodrum</t>
+          <t>2. Kat</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>07-11-2024</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-yigitler-kiralik/daire/122602-100</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-gaziler-kiralik/daire/25220-2509</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -997,58 +982,58 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>FOR SALE &amp; FOR RENTTEN 3+1 VALİ RAHMİ BEY MAH 150 M2 ARA KAT DAİRE</t>
+          <t>ARGA'DAN BUCA 9 EYLÜL İİBF YAKIN 2+0 60m2 EŞYALI KİRALIK DAİRE.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Vali Rahmi Bey Mah.</t>
+          <t>İzmir / Buca / Adatepe Mah.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>25.000
+          <t>16.500
 TL</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>155 m²</t>
+          <t>65 m²</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>25 Yaşında</t>
+          <t>6 Yaşında</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3. Kat</t>
+          <t>Ara Kat</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>06-11-2024</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-vali-rahmi-bey-kiralik/daire/32982-4460</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/63598-162</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Doğalgaz Sobası</t>
+          <t>Kombi</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1060,17 +1045,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GENİŞ, 2 ODA 1 SALON BAHÇELİ YÜKSEK ZEMİN</t>
+          <t>Buca Yeşilbağlar Mh. 2+1 Kapalı Mutfak 110 M2 Kiralık Daire</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Efeler Mah.</t>
+          <t>İzmir / Buca / Yeşilbağlar Mah.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>15.000
+          <t>12.500
 TL</t>
         </is>
       </c>
@@ -1081,12 +1066,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>109 m²</t>
+          <t>110 m²</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>29 Yaşında</t>
+          <t>30 Yaşında</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1096,12 +1081,12 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>05-11-2024</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-efeler-kiralik/daire/13470-2483</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-yesilbaglar-kiralik/daire/24511-9150</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1111,7 +1096,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Isıtma Yok</t>
+          <t>Klima</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1123,48 +1108,48 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Buca Yedigöller 2+1 85 M2 D.gazlı Arakat Kiralık Daire</t>
+          <t>Bucanın Gözbebeği Yeşilbağlarda Havuzlu Sitede 3+1 Kiralık Daire</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Çağdaş Mah.</t>
+          <t>İzmir / Buca / Yeşilbağlar Mah.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>17.000
+          <t>32.000
 TL</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>85 m²</t>
+          <t>160 m²</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>25 Yaşında</t>
+          <t>11 Yaşında</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2. Kat</t>
+          <t>3. Kat</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>05-11-2024</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-cagdas-kiralik/daire/83461-473</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-yesilbaglar-kiralik/daire/123628-20</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1174,60 +1159,55 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Klima</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
+          <t>Kombi</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>FOR SALE &amp; FOR RENTTEN 3+1 İNKİLAPTA 150M2  ŞİRİNYER METRO YAKINI SON KAT DAİRE</t>
+          <t>GÜNEŞ EMLAK'TAN FORBES YAKINI 1+1 OTOPARKLI LÜKS SIFIR DAİRE</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>İzmir / Buca / İnkılap Mah.</t>
+          <t>İzmir / Buca / Yiğitler Mah.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>21.000
+          <t>17.000
 TL</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>160 m²</t>
+          <t>50 m²</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>25 Yaşında</t>
+          <t>Sıfır Bina</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>En Üst Kat</t>
+          <t>Yüksek Giriş</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>05-11-2024</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-inkilap-kiralik/daire/32982-4450</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-yigitler-kiralik/daire/130324-810</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1249,111 +1229,116 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MARKA'DAN H.AĞA BAHÇESİ YAKINI 1+0 EŞYALI KİRALIK DAİRE</t>
+          <t>İZMİR BUCA BUCAKOOP</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Adatepe Mah.</t>
+          <t>İzmir / Buca / Buca Koop. Mah.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>11.000
+          <t>22.000
 TL</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Stüdyo</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>45 m²</t>
+          <t>120 m²</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2 Yaşında</t>
+          <t>25 Yaşında</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Yüksek Giriş</t>
+          <t>7. Kat</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>04-11-2024</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/71024-1052</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Eşyalı</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-buca-koop-kiralik/daire/37745-1879</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Isıtma Yok</t>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>--DOĞALGAZLI-ARAKAT-Buca-doğum hastanesi YAKINI - 3+1-125M2</t>
+          <t>BUCA ŞİRİNYER İZBAN YAKININDA 1+1 50M2 DOĞALGAZLI ULTRA LÜKS EMSALSİZ SIFIR KİRALIK DAİRE</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Atatürk Mah.</t>
+          <t>İzmir / Buca / Akıncılar Mah.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>19.000
+          <t>16.500
 TL</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>125 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>13 Yaşında</t>
+          <t>Sıfır Bina</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Ara Kat</t>
+          <t>Bahçe Katı</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>04-11-2024</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/13470-169</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-akincilar-kiralik/daire/133137-601</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Isıtma Yok</t>
+          <t>Kombi</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1365,169 +1350,169 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Buca Çevik-1 Pazaryeri Çift Cepheli 2+1 Ayrı Mutfaklı 115m2 Ön ve Arka Balkonlu ESNAFOĞLU'ndan</t>
+          <t>Buca Göksu Mah. 1+1 Kiralık Daire</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kozağaç Mah.</t>
+          <t>İzmir / Buca / Göksu Mah.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>18.000
+          <t>12.000
 TL</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>120 m²</t>
+          <t>90 m²</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>20 Yaşında</t>
+          <t>25 Yaşında</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2. Kat</t>
+          <t>1. Kat</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>05-11-2024</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kozagac-kiralik/daire/67273-3993</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-goksu-kiralik/daire/134354-1443</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
           <t>Kombi</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MARKA'DAN ANACADDE&amp;KAMPÜS YAKINI 1+1 EŞYALI ARAKAT KİRALIK DAİRE</t>
+          <t>ONE HOUSE GAYRİMENKUL’DEN DUMLUPINAR MAHALLESİNDE 3+1 GENİŞ DAİRE</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+          <t>İzmir / Buca / Dumlupınar Mah.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>12.500
+          <t>22.000
 TL</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>55 m²</t>
+          <t>145 m²</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>21 Yaşında</t>
+          <t>12 Yaşında</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2. Kat</t>
+          <t>En Üst Kat</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>04-11-2024</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/71024-1051</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-dumlupinar-kiralik/daire/144273-127</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
           <t>Klima</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Elektrik</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GOLDİA YAPI'DAN KAMPÜS YAKINI KİRALIK 1+1 DAİRE !!!</t>
+          <t>PARİSA'DN FUL EŞYALI D.GAZLI KLİMALI 8-9-10-11 AYLIK KISMİ DÖNEM</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Adatepe Mah.</t>
+          <t>İzmir / Buca / Kuruçeşme Mah.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>16.000
+          <t>14.500
 TL</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>Stüdyo</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>50 m²</t>
+          <t>48 m²</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>3 Yaşında</t>
+          <t>5 Yaşında</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>3. Kat</t>
+          <t>1. Kat</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>10-11-2024</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/142618-218</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/143816-43</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1538,86 +1523,86 @@
       <c r="K18" t="inlineStr">
         <is>
           <t>Kombi</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MARKA'DAN ANACADDE&amp;KAMPÜS YAKINI 1+1 KLİMALI KİRALIK DAİRE</t>
+          <t>Kiralık Site İçinde Büyük Arakat Daire</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+          <t>İzmir / Buca / Buca Koop. Mah.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>13.000
+          <t>28.000
 TL</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>50 m²</t>
+          <t>150 m²</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>4 Yaşında</t>
+          <t>18 Yaşında</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Yüksek Giriş</t>
+          <t>6. Kat</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>04-11-2024</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/71024-1049</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-buca-koop-kiralik/daire/82933-244</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Klima</t>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MARKA'DAN ANACADDE&amp;KAMPÜS YAKINI EŞYALI KLİMALI KİRALIK DAİRE</t>
+          <t>Tınaztepe kampüse yürüyerek 10 dk mesafede eşyalı ev</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+          <t>İzmir / Buca / Atatürk Mah.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>15.000
+          <t>18.500
 TL</t>
         </is>
       </c>
@@ -1628,27 +1613,27 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>55 m²</t>
+          <t>50 m²</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2 Yaşında</t>
+          <t>4 Yaşında</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2. Kat</t>
+          <t>6. Kat</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>07-11-2024</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/71024-1048</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/141901-213</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1659,117 +1644,127 @@
       <c r="K20" t="inlineStr">
         <is>
           <t>Klima</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Elektrik</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ATATÜRK MAH'DE SİTE İÇİ ARA KAT D. GAZLI FULL EŞYALI 1+1 DAİRE</t>
+          <t>SİTE İÇİ KİRALIK 3+1 145m2 ARAKAT DAİRE</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Atatürk Mah.</t>
+          <t>İzmir / Buca / Mustafa Kemal Mah.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>17.000
+          <t>33.500
 TL</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>55 m²</t>
+          <t>145 m²</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>5 Yaşında</t>
+          <t>3 Yaşında</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>5. Kat</t>
+          <t>12. Kat</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>18-10-2024</t>
+          <t>08-11-2024</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/142478-123</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-mustafa-kemal-kiralik/daire/145608-91</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
           <t>Merkezi (Pay Ölçer)</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BUCA ATATÜRK MAHALLESİNDE 3+1 FULL TADİLATLI MERKEZİ KONUM ULAŞIMI 4 BALKONLU KİRALIK DAİRE</t>
+          <t>GOLDİA YAPI'DAN KAMPÜS YAKINI KİRALIK 1+1 DAİRE</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Atatürk Mah.</t>
+          <t>İzmir / Buca / Adatepe Mah.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>20.000
+          <t>17.000
 TL</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>130 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>15 Yaşında</t>
+          <t>3 Yaşında</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>En Üst Kat</t>
+          <t>2. Kat</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>17-10-2024</t>
+          <t>05-11-2024</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/150876-20</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/142618-249</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1786,80 +1781,75 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Şirinyer Güven Mh. 3+1 145 M2 Doğalgazlı Arakat Kiralık Daire</t>
+          <t>EŞYALI KLİMALI BALKONLU 8-9-10-11 AYLIK KISMİ DÖNEMLİ KİRALAMA</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Güven Mah.</t>
+          <t>İzmir / Buca / Kuruçeşme Mah.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>21.500
+          <t>10.500
 TL</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>Stüdyo</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>145 m²</t>
+          <t>48 m²</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>20 Yaşında</t>
+          <t>5 Yaşında</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>3. Kat</t>
+          <t>1. Kat</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>17-10-2024</t>
+          <t>10-11-2024</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-guven-kiralik/daire/24511-9109</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/143816-42</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Kombi</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
+          <t>Klima</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ARGA'DAN BUCA ŞİRİNYER'DE 3+1 EŞYALI DOĞALGAZLI KİRALIK DAİRE.</t>
+          <t>ARGA'DAN BUCA ÇEVİK BİR'DE 3+1 ARAKAT KİRALIK DAİRE</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Yiğitler Mah.</t>
+          <t>İzmir / Buca / Kozağaç Mah.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>22.000
+          <t>23.000
 TL</t>
         </is>
       </c>
@@ -1870,90 +1860,85 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>135 m²</t>
+          <t>130 m²</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>27 Yaşında</t>
+          <t>30 Yaşında</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Ara Kat</t>
+          <t>3. Kat</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>17-10-2024</t>
+          <t>09-11-2024</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-yigitler-kiralik/daire/63598-149</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-kozagac-kiralik/daire/63598-132</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
           <t>Kombi</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ÜNİVERSİTE KARŞISI ARAKAT DOĞALGAZLI SIFIR LÜX EŞYALI  KİRALIK DAİRE</t>
+          <t>EŞYALI-BUCA HASANAĞA -1 ODA 1 SALON Açık Mutfaklı</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+          <t>İzmir / Buca / Dumlupınar Mah.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>35.000
+          <t>18.500
 TL</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>130 m²</t>
+          <t>60 m²</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>5 Yaşında</t>
+          <t>11 Yaşında</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Ara Kat</t>
+          <t>2. Kat</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>16-10-2024</t>
+          <t>05-11-2024</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/0-43551010</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-dumlupinar-kiralik/daire/13470-1741</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -1963,45 +1948,45 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Kombi</t>
+          <t>Klima</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Doğalgaz</t>
+          <t>Elektrik</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MENDERES MH.DE 2+1 ÇİFT CEPHE ARAKAT 85 M2 ARAKAT KİRALIK DAİRE</t>
+          <t>AKTİFLER'den Şirinyer'de Otoparklı 3+1 Eşyalı Kiralık Yeni Daire</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Menderes Mah.</t>
+          <t>İzmir / Buca / İnkılap Mah.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>14.000
+          <t>30.000
 TL</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>84 m²</t>
+          <t>130 m²</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>25 Yaşında</t>
+          <t>12 Yaşında</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2011,12 +1996,12 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>08-11-2024</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-menderes-kiralik/daire/147777-163</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-inkilap-kiralik/daire/21865-5172</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2038,12 +2023,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Menderes Mh. Öğrenciye Kiralık 4+1 130 M2 Teraslı Doğalgazlı Daire</t>
+          <t>Kiralık 3+1 Arakat Doğalgazlı</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Menderes Mah.</t>
+          <t>İzmir / Buca / Hürriyet Mah.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2054,12 +2039,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>4 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>130 m²</t>
+          <t>120 m²</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2069,17 +2054,17 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2. Kat</t>
+          <t>3. Kat</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>26-09-2024</t>
+          <t>04-11-2024</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-menderes-kiralik/daire/24511-9074</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-hurriyet-kiralik/daire/82933-241</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2089,7 +2074,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Merkezi (Pay Ölçer)</t>
+          <t>Kombi</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2101,17 +2086,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Buca Göksu Mah İnkılap İzban Dibi 3+1 120 M2 D.gazlı</t>
+          <t>Buca da Şirinyer Hürriyet mahallesinde Kiralık 3+1 Dığalgazlı daire</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Göksu Mah.</t>
+          <t>İzmir / Buca / Hürriyet Mah.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>14.000
+          <t>17.000
 TL</t>
         </is>
       </c>
@@ -2122,27 +2107,32 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>120 m²</t>
+          <t>140 m²</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>21 Yaşında</t>
+          <t>35 Yaşında</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Giriş Katı</t>
+          <t>En Üst Kat</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>08-11-2024</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-goksu-kiralik/daire/83461-581</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-hurriyet-kiralik/daire/122602-144</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2159,17 +2149,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GÜNEŞ'TEN ŞİRİNYER İZBAN 9DK 1+1 50M ASANSÖR KLİMA GÜNEY CEPHE</t>
+          <t>Buca Kuruçeşme’de, Tınaztepe Hastanesi’nin Yanında, 1+1 Kiralık Daire</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>İzmir / Buca / İnkılap Mah.</t>
+          <t>İzmir / Buca / Kuruçeşme Mah.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16.500
+          <t>15.000
 TL</t>
         </is>
       </c>
@@ -2180,27 +2170,27 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>49 m²</t>
+          <t>60 m²</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2 Yaşında</t>
+          <t>11 Yaşında</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>4. Kat</t>
+          <t>1. Kat</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>06-11-2024</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-inkilap-kiralik/daire/130324-802</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/126264-1847</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2222,48 +2212,48 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SİTE İÇİ KİRALIK 3+1 145m2 ARAKAT DAİRE</t>
+          <t>TINAZTEPE HASTANESİ KARŞISI 1+1 EŞYALI KİRALIK DAİRE</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Mustafa Kemal Mah.</t>
+          <t>İzmir / Buca / Kuruçeşme Mah.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>34.000
+          <t>15.500
 TL</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>145 m²</t>
+          <t>60 m²</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>3 Yaşında</t>
+          <t>11 Yaşında</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>12. Kat</t>
+          <t>3. Kat</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>06-11-2024</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-mustafa-kemal-kiralik/daire/145608-91</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/120563-1814</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2285,53 +2275,53 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Deniz emlak dan Buca'da Yenigün mahallesinde kiralık daire</t>
+          <t>Şirinyer Yiğitler Mh 1+1 Sıfır Asansörlü Doğalgazlı Kiralık Daire</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kozağaç Mah.</t>
+          <t>İzmir / Buca / Yiğitler Mah.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>15.000
+          <t>18.000
 TL</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>130 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>16 Yaşında</t>
+          <t>Sıfır Bina</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>4. Kat</t>
+          <t>Yüksek Giriş</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>07-11-2024</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kozagac-kiralik/daire/120009-3</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-yigitler-kiralik/daire/24511-9156</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2348,75 +2338,75 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>BUCADA EŞYALI, ASANSÖRLÜ, DOĞALGAZLI,KLİMALI, DOKUZ EYLÜL ÜNİ YANI, 1+1 KİRALIK</t>
+          <t>BUCA İZBAN YAKINI 2+1 bahçeli yüksek giriş kiralık daire</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+          <t>İzmir / Buca / İnkılap Mah.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>25.000
+          <t>18.000
 TL</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>2 + 1</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>50 m²</t>
+          <t>75 m²</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>4 Yaşında</t>
+          <t>3 Yaşında</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>8. Kat</t>
+          <t>Yüksek Giriş</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>08-11-2024</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/77173-1070</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>Eşyalı</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-inkilap-kiralik/daire/16596-1218</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Klima</t>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Kiralık Buca da Yiğitler Mah.3+1 110 m2 Doğalgazlı açık otoparkı olan merkez de bir daire</t>
+          <t>BUCA FIRAT MAH. 3+1 125 M2 AÇIK MUTFAK DOĞALGAZLI KİRALIK DAİRE</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Yiğitler Mah.</t>
+          <t>İzmir / Buca / Fırat Mah.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>20.000
+          <t>19.000
 TL</t>
         </is>
       </c>
@@ -2427,27 +2417,27 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>110 m²</t>
+          <t>130 m²</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>7 Yaşında</t>
+          <t>15 Yaşında</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Yarı Bodrum</t>
+          <t>Ara Kat</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>04-11-2024</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-yigitler-kiralik/daire/122602-100</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-firat-kiralik/daire/64940-53</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2469,58 +2459,58 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>FOR SALE &amp; FOR RENTTEN 3+1 VALİ RAHMİ BEY MAH 150 M2 ARA KAT DAİRE</t>
+          <t>bucaPARİSA'DAN TINAZTEPE KAMP.KARŞISI D.GAZLI EŞYALI KİRALIK 1+1</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Vali Rahmi Bey Mah.</t>
+          <t>İzmir / Buca / Kuruçeşme Mah.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>25.000
+          <t>15.000
 TL</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>155 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>25 Yaşında</t>
+          <t>10 Yaşında</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>3. Kat</t>
+          <t>2. Kat</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>10-11-2024</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-vali-rahmi-bey-kiralik/daire/32982-4460</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/143816-27</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Merkezi (Pay Ölçer)</t>
+          <t>Kombi</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2532,191 +2522,186 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GENİŞ, 2 ODA 1 SALON BAHÇELİ YÜKSEK ZEMİN</t>
+          <t>İNÖNÜ MAH. SIFIR 1+1 KİRALIK DUBLEKS</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Efeler Mah.</t>
+          <t>İzmir / Buca / İnönü Mah.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15.000
+          <t>13.000
 TL</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>109 m²</t>
+          <t>70 m²</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>29 Yaşında</t>
+          <t>Sıfır Bina</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Yüksek Giriş</t>
+          <t>1. Kat</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>07-11-2024</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-efeler-kiralik/daire/13470-2483</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-inonu-kiralik/daire/141901-220</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Merkezi (Pay Ölçer)</t>
+          <t>Isıtma Yok</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Buca Yedigöller 2+1 85 M2 D.gazlı Arakat Kiralık Daire</t>
+          <t>ÖZPA - ŞİRİNYER İZBANDA DOĞALGAZLI AÇIK OTOPARKLI  TEMİZ 1+1 KİRALIK DAİRE</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Çağdaş Mah.</t>
+          <t>İzmir / Buca / Hürriyet Mah.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>17.000
+          <t>15.000
 TL</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>85 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>25 Yaşında</t>
+          <t>4 Yaşında</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2. Kat</t>
+          <t>3. Kat</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>06-11-2024</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-cagdas-kiralik/daire/83461-473</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-hurriyet-kiralik/daire/25220-1898</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Klima</t>
+          <t>Kombi</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Elektrik</t>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>FOR SALE &amp; FOR RENTTEN 3+1 İNKİLAPTA 150M2  ŞİRİNYER METRO YAKINI SON KAT DAİRE</t>
+          <t>BUCA KURUÇEŞME MEYDAN'DA FULL EŞYALI YÜKSEK GİRİŞ</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>İzmir / Buca / İnkılap Mah.</t>
+          <t>İzmir / Buca / Kuruçeşme Mah.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>21.000
+          <t>16.000
 TL</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>160 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>25 Yaşında</t>
+          <t>1 Yaşında</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>En Üst Kat</t>
+          <t>Yüksek Giriş</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>06-11-2024</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-inkilap-kiralik/daire/32982-4450</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/142618-136</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Kombi</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
+          <t>Klima</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>MARKA'DAN H.AĞA BAHÇESİ YAKINI 1+0 EŞYALI KİRALIK DAİRE</t>
+          <t>BUCA KONFORUN ADRESİ</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2726,18 +2711,18 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>11.000
+          <t>200
 TL</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Stüdyo</t>
+          <t>2 + 1</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>45 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2747,49 +2732,39 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Yüksek Giriş</t>
+          <t>Ara Kat</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>10-11-2024</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/71024-1052</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>Eşyalı</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/138098-14</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Kombi</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
+          <t>Klima</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>--DOĞALGAZLI-ARAKAT-Buca-doğum hastanesi YAKINI - 3+1-125M2</t>
+          <t>AKTİFLER'den Buca Şirinyer'de Eşyalı Kiralık Otoparklı Köşe Daire</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Atatürk Mah.</t>
+          <t>İzmir / Buca / İnkılap Mah.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>19.000
+          <t>21.500
 TL</t>
         </is>
       </c>
@@ -2800,54 +2775,59 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>125 m²</t>
+          <t>120 m²</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>13 Yaşında</t>
+          <t>35 Yaşında</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Ara Kat</t>
+          <t>3. Kat</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>06-11-2024</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/13470-169</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-inkilap-kiralik/daire/21865-5147</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Klima</t>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Buca Çevik-1 Pazaryeri Çift Cepheli 2+1 Ayrı Mutfaklı 115m2 Ön ve Arka Balkonlu ESNAFOĞLU'ndan</t>
+          <t>GENİŞ, 2 ODA 1 SALON BAHÇELİ YÜKSEK ZEMİN</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kozağaç Mah.</t>
+          <t>İzmir / Buca / Efeler Mah.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>18.000
+          <t>13.500
 TL</t>
         </is>
       </c>
@@ -2858,27 +2838,27 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>120 m²</t>
+          <t>109 m²</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>20 Yaşında</t>
+          <t>29 Yaşında</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2. Kat</t>
+          <t>Yüksek Giriş</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>08-11-2024</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kozagac-kiralik/daire/67273-3993</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-efeler-kiralik/daire/13470-2483</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -2888,65 +2868,65 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Kombi</t>
+          <t>Isıtma Yok</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Doğalgaz</t>
+          <t>Elektrik</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>MARKA'DAN ANACADDE&amp;KAMPÜS YAKINI 1+1 EŞYALI ARAKAT KİRALIK DAİRE</t>
+          <t>YAYLACIK MAH 3+1 EŞYALI GİRİŞ KATI DAİRE</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+          <t>İzmir / Buca / Yaylacık Mah.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>12.500
+          <t>25.000
 TL</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>55 m²</t>
+          <t>130 m²</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>21 Yaşında</t>
+          <t>20 Yaşında</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2. Kat</t>
+          <t>Giriş Katı</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>10-11-2024</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/71024-1051</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-yaylacik-kiralik/daire/14003-1500</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -2963,154 +2943,149 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>GOLDİA YAPI'DAN KAMPÜS YAKINI KİRALIK 1+1 DAİRE !!!</t>
+          <t>BUCA MUSTAFA KEMALDE KİRALIK ARAKAT DAİRE 110 m2 2+1 KAT 2</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Adatepe Mah.</t>
+          <t>İzmir / Buca / Mustafa Kemal Mah.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16.000
+          <t>11.000
 TL</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>2 + 1</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>50 m²</t>
+          <t>110 m²</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>3 Yaşında</t>
+          <t>11 Yaşında</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>3. Kat</t>
+          <t>2. Kat</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>08-11-2024</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/142618-218</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-mustafa-kemal-kiralik/daire/149571-8</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Kombi</t>
+          <t>Soba</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MARKA'DAN ANACADDE&amp;KAMPÜS YAKINI 1+1 KLİMALI KİRALIK DAİRE</t>
+          <t>KAMU PERSONELİ AİLEYE EŞYALI&amp;EŞYASIZ DOĞALGAZLI KİRALIK DAİRE</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+          <t>İzmir / Buca / Yeşilbağlar Mah.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>13.000
+          <t>17.500
 TL</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>2 + 1</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>50 m²</t>
+          <t>100 m²</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>4 Yaşında</t>
+          <t>21 Yaşında</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Yüksek Giriş</t>
+          <t>4. Kat</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>04-11-2024</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/71024-1049</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-yesilbaglar-kiralik/daire/140664-80</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
           <t>Kombi</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MARKA'DAN ANACADDE&amp;KAMPÜS YAKINI EŞYALI KLİMALI KİRALIK DAİRE</t>
+          <t>VALİ RAHMİ BEY MAHALLESİNDE GENİŞ 2+1 FULL EŞYALI KİRALIK DAİRE</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+          <t>İzmir / Buca / Efeler Mah.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15.000
+          <t>24.000
 TL</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>2 + 1</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>55 m²</t>
+          <t>120 m²</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2 Yaşında</t>
+          <t>31 Yaşında</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -3120,17 +3095,17 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>07-11-2024</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/71024-1048</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-efeler-kiralik/daire/143815-155</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3147,48 +3122,48 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ATATÜRK MAH'DE SİTE İÇİ ARA KAT D. GAZLI FULL EŞYALI 1+1 DAİRE</t>
+          <t>Buca Şirinyer İzban Arkası/Nato Karşısı Eşyalı 3+1 Arakat Daire</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Atatürk Mah.</t>
+          <t>İzmir / Buca / İnkılap Mah.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>17.000
+          <t>23.000
 TL</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>55 m²</t>
+          <t>125 m²</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>5 Yaşında</t>
+          <t>25 Yaşında</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>5. Kat</t>
+          <t>2. Kat</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>18-10-2024</t>
+          <t>07-11-2024</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/142478-123</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-inkilap-kiralik/daire/24511-9159</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -3198,14 +3173,19 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Merkezi (Pay Ölçer)</t>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>BUCA ATATÜRK MAHALLESİNDE 3+1 FULL TADİLATLI MERKEZİ KONUM ULAŞIMI 4 BALKONLU KİRALIK DAİRE</t>
+          <t>Buca Atatürk Mahallesi Klimalı Ultra Lüks Eşyalı 1+1............</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3215,38 +3195,38 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>20.000
+          <t>15.500
 TL</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>130 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>15 Yaşında</t>
+          <t>9 Yaşında</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>En Üst Kat</t>
+          <t>3. Kat</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>17-10-2024</t>
+          <t>09-11-2024</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/150876-20</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/151862-13</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3258,91 +3238,96 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Şirinyer Güven Mh. 3+1 145 M2 Doğalgazlı Arakat Kiralık Daire</t>
+          <t>ADATEPE MAHALLESİ FULL EŞYALI DOĞALGAZLI KİRALIK 1+1</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Güven Mah.</t>
+          <t>İzmir / Buca / Adatepe Mah.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>21.500
+          <t>17.000
 TL</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>145 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>20 Yaşında</t>
+          <t>4 Yaşında</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>3. Kat</t>
+          <t>1. Kat</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>17-10-2024</t>
+          <t>06-11-2024</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-guven-kiralik/daire/24511-9109</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/150997-1</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
           <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ARGA'DAN BUCA ŞİRİNYER'DE 3+1 EŞYALI DOĞALGAZLI KİRALIK DAİRE.</t>
+          <t>EŞYALI-DOĞALGAZLI 2 ODA 1 SALON-ARAKAT DAİRE</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Yiğitler Mah.</t>
+          <t>İzmir / Buca / Kozağaç Mah.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>22.000
+          <t>18.000
 TL</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>2 + 1</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>135 m²</t>
+          <t>80 m²</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>27 Yaşında</t>
+          <t>5 Yaşında</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -3352,12 +3337,12 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>17-10-2024</t>
+          <t>09-11-2024</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-yigitler-kiralik/daire/63598-149</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-kozagac-kiralik/daire/13470-2474</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3379,17 +3364,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ÜNİVERSİTE KARŞISI ARAKAT DOĞALGAZLI SIFIR LÜX EŞYALI  KİRALIK DAİRE</t>
+          <t>2+1 KAMPÜS YAKINI GENİŞ DAİRE</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+          <t>İzmir / Buca / Atatürk Mah.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>35.000
+          <t>20.000
 TL</t>
         </is>
       </c>
@@ -3400,32 +3385,32 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>130 m²</t>
+          <t>75 m²</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>5 Yaşında</t>
+          <t>10 Yaşında</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Ara Kat</t>
+          <t>Yüksek Giriş</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>16-10-2024</t>
+          <t>07-11-2024</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/0-43551010</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/147777-164</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -3442,53 +3427,53 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>MENDERES MH.DE 2+1 ÇİFT CEPHE ARAKAT 85 M2 ARAKAT KİRALIK DAİRE</t>
+          <t>Sahibinden Kiralık Şirinyer İzban Meydanı Eşyalı 1+1</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Menderes Mah.</t>
+          <t>İzmir / Buca / İnkılap Mah.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>14.000
+          <t>25.000
 TL</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>84 m²</t>
+          <t>50 m²</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>25 Yaşında</t>
+          <t>4 Yaşında</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2. Kat</t>
+          <t>En Üst Kat</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>08-11-2024</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-menderes-kiralik/daire/147777-163</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-inkilap-kiralik/daire/0-43668227</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -3505,33 +3490,33 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Menderes Mh. Öğrenciye Kiralık 4+1 130 M2 Teraslı Doğalgazlı Daire</t>
+          <t>Buca Yaylacık'ta İster Eşyasız İster Eşyalı 3+1 Ebeveynli 2 Balkonlu Kiler v Otoparklı ESNAFOĞLU'nda</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Menderes Mah.</t>
+          <t>İzmir / Buca / Yaylacık Mah.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>20.000
+          <t>18.000
 TL</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>4 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>130 m²</t>
+          <t>150 m²</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>25 Yaşında</t>
+          <t>20 Yaşında</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -3541,75 +3526,70 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>26-09-2024</t>
+          <t>07-11-2024</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-menderes-kiralik/daire/24511-9074</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>Eşyalı</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-yaylacik-kiralik/daire/67273-3998</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Klima</t>
+          <t>Kombi</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Elektrik</t>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Buca Göksu Mah İnkılap İzban Dibi 3+1 120 M2 D.gazlı</t>
+          <t>TINAZTEPE KAMPÜS KARŞISINDA 2+0  EŞYASIZ KİRALIK DAİRE</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Göksu Mah.</t>
+          <t>İzmir / Buca / Kuruçeşme Mah.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>14.000
+          <t>15.000
 TL</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>2 + 1</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>120 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>21 Yaşında</t>
+          <t>8 Yaşında</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Giriş Katı</t>
+          <t>Ara Kat</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>10-11-2024</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-goksu-kiralik/daire/83461-581</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/150707-9</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -3631,133 +3611,133 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>GÜNEŞ'TEN ŞİRİNYER İZBAN 9DK 1+1 50M ASANSÖR KLİMA GÜNEY CEPHE</t>
+          <t>BUCA GÖKSUDA İNKILAP İZBAN YAKINI KİRALIK 2+1 YÜKSEK GİRİŞ</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>İzmir / Buca / İnkılap Mah.</t>
+          <t>İzmir / Buca / Göksu Mah.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16.500
+          <t>11.000
 TL</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>2 + 1</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>49 m²</t>
+          <t>85 m²</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2 Yaşında</t>
+          <t>4 Yaşında</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>4. Kat</t>
+          <t>Yüksek Giriş</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>08-11-2024</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-inkilap-kiralik/daire/130324-802</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-goksu-kiralik/daire/149571-7</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Kombi</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>Doğalgaz</t>
+          <t>Isıtma Yok</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>SİTE İÇİ KİRALIK 3+1 145m2 ARAKAT DAİRE</t>
+          <t>GÜNEŞ'TEN ŞİRNYER METRO 5DK 2+1 90M 3.KAT BALKON</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Mustafa Kemal Mah.</t>
+          <t>İzmir / Buca / Hürriyet Mah.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>34.000
+          <t>16.000
 TL</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>2 + 1</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>145 m²</t>
+          <t>90 m²</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>3 Yaşında</t>
+          <t>40 Yaşında</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>12. Kat</t>
+          <t>3. Kat</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>10-11-2024</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-mustafa-kemal-kiralik/daire/145608-91</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-hurriyet-kiralik/daire/130324-747</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Eşyalı</t>
+          <t>Eşyalı Değil</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Klima</t>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Deniz emlak dan Buca'da Yenigün mahallesinde kiralık daire</t>
+          <t>AKTİFLER'den Buca Adatepe'de 1+1 Eşyalı Kiralık Yeni Daire</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kozağaç Mah.</t>
+          <t>İzmir / Buca / Adatepe Mah.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3768,32 +3748,32 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>1 + 1</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>130 m²</t>
+          <t>55 m²</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>16 Yaşında</t>
+          <t>6 Yaşında</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>4. Kat</t>
+          <t>2. Kat</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>07-11-2024</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kozagac-kiralik/daire/120009-3</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/21865-5164</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -3803,133 +3783,1106 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Merkezi (Pay Ölçer)</t>
+          <t>Klima</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Elektrik</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>BUCADA EŞYALI, ASANSÖRLÜ, DOĞALGAZLI,KLİMALI, DOKUZ EYLÜL ÜNİ YANI, 1+1 KİRALIK</t>
+          <t>İBF' YE YÜRÜME MESAFESİNDE  TERASLI GENİŞ FERAH KİRALIK DAİRE !!</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+          <t>İzmir / Buca / Adatepe Mah.</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>25.000
+          <t>21.000
 TL</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>2 + 1</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>50 m²</t>
+          <t>150 m²</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>4 Yaşında</t>
+          <t>8 Yaşında</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>8. Kat</t>
+          <t>En Üst Kat</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>19-10-2024</t>
+          <t>06-11-2024</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/77173-1070</t>
+          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/150997-2</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Eşyalı Değil</t>
+          <t>Eşyalı</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Klima</t>
+          <t>Kombi</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Kömür-Odun</t>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Kiralık Buca da Yiğitler Mah.3+1 110 m2 Doğalgazlı açık otoparkı olan merkez de bir daire</t>
+          <t>MARKA'DAN ANACADDE&amp;KAMPÜS YAKINI 1+1 EŞYALI&amp;KLİMALI KİRALIK DAİR</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>İzmir / Buca / Yiğitler Mah.</t>
+          <t>İzmir / Buca / Atatürk Mah.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
+          <t>15.000
+TL</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>1 + 1</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>55 m²</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>4 Yaşında</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2. Kat</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>09-11-2024</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/71024-1091</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Eşyalı</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Klima</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>BUCA YEŞİLBAĞLARDA KİRALIK GIRIŞKAT 2+1 DAİRE</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Yeşilbağlar Mah.</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>15.000
+TL</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2 + 1</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>100 m²</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>16 Yaşında</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Giriş Katı</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>08-11-2024</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-yesilbaglar-kiralik/daire/149571-6</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Eşyalı Değil</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Isıtma Yok</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ARGA'DAN BUCA FIRAT MAH, D.GAZLI ARA KAT 3+1 KİRALIK DAİRE.</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Fırat Mah.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>22.000
+TL</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>3 + 1</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>130 m²</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>22 Yaşında</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Ara Kat</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>09-11-2024</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-firat-kiralik/daire/63598-158</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Eşyalı Değil</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ATA EMLKTAN ŞİRİNYER İZBAN YK GENİŞ 3+1 DAİRE</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Hürriyet Mah.</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>20.500
+TL</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>3 + 2</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>140 m²</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>41 Yaşında</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>En Üst Kat</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>05-11-2024</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-hurriyet-kiralik/daire/6425-4608</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Eşyalı</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>BUCA KAMPÜS YAKINI 1+0 EŞYALI KİRALIK DAİRE</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Adatepe Mah.</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>11.000
+TL</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Stüdyo</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>40 m²</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>9 Yaşında</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>3. Kat</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>09-11-2024</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/109132-312</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Eşyalı</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Klima</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Elektrik</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Buca Çevik-1'de Çift Cepheli Sıfır 2+1 Balkonlu Otoparklı Asansörlü ESNAFOĞLU'ndan..</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Kozağaç Mah.</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
           <t>20.000
 TL</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2 + 1</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>85 m²</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Sıfır Bina</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>3. Kat</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>07-11-2024</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-kozagac-kiralik/daire/67273-3995</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Eşyalı Değil</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>LORA’DAN ATATÜRK MAHALLESİ SIFIR EŞYALI DOĞALGAZLI ARAKAT</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Atatürk Mah.</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>20.000
+TL</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>1 + 1</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>50 m²</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Sıfır Bina</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2. Kat</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>08-11-2024</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/150727-5</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Eşyalı</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>BUCA ATATÜRK MAHALLESİNDE ÜNİVERSİTEYE YAKIN 2+0 GAYET KULLANIŞLI DOĞALGAZLI ARAKAT KİRALIK DAİRE</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Atatürk Mah.</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>18.500
+TL</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2 + 1</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>75 m²</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Sıfır Bina</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Ara Kat</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>08-11-2024</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-ataturk-kiralik/daire/150876-5</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Eşyalı Değil</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>ONE HOUSE’DAN ADATEPE MAHALLESİNDE 1+1 EŞYALI DAİRE</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Adatepe Mah.</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>16.000
+TL</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>1 + 1</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>47 m²</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>7 Yaşında</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Ara Kat</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>06-11-2024</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/144273-130</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Eşyalı</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>BUCA GÖKSUDA KİRALIK DOĞALGAZLI 3+1 DAİRE</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Göksu Mah.</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>15.000
+TL</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
         <is>
           <t>3 + 1</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>110 m²</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>7 Yaşında</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Yarı Bodrum</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>19-10-2024</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>https://www.hepsiemlak.com/izmir-buca-yigitler-kiralik/daire/122602-100</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>140 m²</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>11 Yaşında</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>4. Kat</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>08-11-2024</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-goksu-kiralik/daire/149571-5</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
         <is>
           <t>Eşyalı Değil</t>
         </is>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>Soba</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>Kömür-Odun</t>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>MARKA'DAN ANACADDE&amp;KAMPÜS YAKINI EŞYALI KLİMALI KİRALIK DAİRE</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Kozağaç Mah.</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>13.000
+TL</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>1 + 1</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>55 m²</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>4 Yaşında</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2. Kat</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>09-11-2024</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-kozagac-kiralik/daire/71024-1088</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Eşyalı</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Klima</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Buca Kozağaç Mah. 2+1 95 M2 Doğalgazlı Kapalı Mutfak Kiralık Daire</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Kozağaç Mah.</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>19.000
+TL</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2 + 1</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>95 m²</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>10 Yaşında</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Kot 1</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>06-11-2024</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-kozagac-kiralik/daire/24511-9152</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Eşyalı Değil</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>bucaPARİSA'DAN KAMPÜS KARŞISI D.GAZLI EŞYALI 1+1</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>15.000
+TL</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>1 + 1</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>55 m²</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>5 Yaşında</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>1. Kat</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>10-11-2024</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/143816-44</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Eşyalı</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Şirinyer Hürriyet Mahallesinde 2+1 Eşyalı Kiralık Daire</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Hürriyet Mah.</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>18.000
+TL</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2 + 1</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>80 m²</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>4 Yaşında</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Ara Kat</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>07-11-2024</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-hurriyet-kiralik/daire/122602-121</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Eşyalı</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>ERA NİVA GAYRİMENKUL 'DEN KİRALIK 2+1 DAİRE</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Kuruçeşme Mah.</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>17.000
+TL</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2 + 1</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>90 m²</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>5 Yaşında</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2. Kat</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>04-11-2024</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-kurucesme-kiralik/daire/140088-487</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Eşyalı Değil</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Buca'da 1750 m2 Arsa İçinde Havuzlu, Eşyalı Lüsk Kiralık Daire</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Karacaağaç Mah.</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>50.000
+TL</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2 + 1</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>1.750 m²</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Sıfır Bina</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>06-11-2024</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-karacaagac-kiralik/villa/151800-4</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Eşyalı</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Hasanağa bahçesi ve üniversiteye yürüme mesafesinde 3+1 site içerisinde kiralık daire</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>İzmir / Buca / Adatepe Mah.</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>25.000
+TL</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>3 + 1</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>130 m²</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>21 Yaşında</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Zemin</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>26-10-2024</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>https://www.hepsiemlak.com/izmir-buca-adatepe-kiralik/daire/139431-31</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Eşyalı Değil</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>Kombi</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Doğalgaz</t>
         </is>
       </c>
     </row>

</xml_diff>